<commit_message>
xlsx written, 2/3 plots done
</commit_message>
<xml_diff>
--- a/TestData/ecom_Lee20220821.xlsx
+++ b/TestData/ecom_Lee20220821.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">dim_deviceCategory</t>
   </si>
@@ -54,6 +54,9 @@
     <t xml:space="preserve">addsToCart</t>
   </si>
   <si>
+    <t xml:space="preserve">transperadd</t>
+  </si>
+  <si>
     <t xml:space="preserve">sess_mom</t>
   </si>
   <si>
@@ -82,27 +85,32 @@
   </si>
   <si>
     <t xml:space="preserve">ECR_momper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transperadd_mom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transperadd_momper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6/2013</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
-  </numFmts>
-  <fonts count="2">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -125,9 +133,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1446,10 +1453,19 @@
       <c r="P1" t="s">
         <v>22</v>
       </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>41395</v>
+      <c r="A2" t="s">
+        <v>26</v>
       </c>
       <c r="B2" t="n">
         <v>1164376</v>
@@ -1466,7 +1482,9 @@
       <c r="F2" t="n">
         <v>0.024381299511498</v>
       </c>
-      <c r="G2"/>
+      <c r="G2" t="n">
+        <v>0.207643358689292</v>
+      </c>
       <c r="H2"/>
       <c r="I2"/>
       <c r="J2"/>
@@ -1476,10 +1494,13 @@
       <c r="N2"/>
       <c r="O2"/>
       <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>41426</v>
+      <c r="A3" t="s">
+        <v>27</v>
       </c>
       <c r="B3" t="n">
         <v>1388516</v>
@@ -1497,34 +1518,43 @@
         <v>0.024874038181771</v>
       </c>
       <c r="G3" t="n">
+        <v>0.319885153283319</v>
+      </c>
+      <c r="H3" t="n">
         <v>224140</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>0.192497955986726</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>6149</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>0.216597978090105</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>10262</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>0.198764260396289</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>-28750</v>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>-0.210283791691047</v>
       </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
         <v>0.000492738670273035</v>
       </c>
-      <c r="P3" t="n">
+      <c r="Q3" t="n">
         <v>0.0202096967817759</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.112241794594027</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.540550852685739</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final code push :)
</commit_message>
<xml_diff>
--- a/TestData/ecom_Lee20220821.xlsx
+++ b/TestData/ecom_Lee20220821.xlsx
@@ -13,15 +13,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">dim_deviceCategory</t>
   </si>
   <si>
-    <t xml:space="preserve">month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">year</t>
+    <t xml:space="preserve">date</t>
   </si>
   <si>
     <t xml:space="preserve">Sessions</t>
@@ -39,6 +36,9 @@
     <t xml:space="preserve">Trans_permonth</t>
   </si>
   <si>
+    <t xml:space="preserve">qty_pertrans</t>
+  </si>
+  <si>
     <t xml:space="preserve">desktop</t>
   </si>
   <si>
@@ -48,9 +48,6 @@
     <t xml:space="preserve">tablet</t>
   </si>
   <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
     <t xml:space="preserve">addsToCart</t>
   </si>
   <si>
@@ -91,26 +88,27 @@
   </si>
   <si>
     <t xml:space="preserve">transperadd_momper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5/2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6/2013</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,8 +131,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,936 +457,936 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="n">
-        <v>7</v>
+      <c r="B2" s="1" t="n">
+        <v>41091</v>
       </c>
       <c r="C2" t="n">
-        <v>2012</v>
+        <v>335226</v>
       </c>
       <c r="D2" t="n">
-        <v>335226</v>
+        <v>10701</v>
       </c>
       <c r="E2" t="n">
-        <v>10701</v>
+        <v>18547</v>
       </c>
       <c r="F2" t="n">
-        <v>18547</v>
+        <v>0.0319217483130783</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0319217483130783</v>
+        <v>0.589229667969825</v>
       </c>
       <c r="H2" t="n">
-        <v>0.589229667969825</v>
+        <v>1.73320250443884</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="n">
-        <v>7</v>
+      <c r="B3" s="1" t="n">
+        <v>41091</v>
       </c>
       <c r="C3" t="n">
-        <v>2012</v>
+        <v>274435</v>
       </c>
       <c r="D3" t="n">
-        <v>274435</v>
+        <v>2576</v>
       </c>
       <c r="E3" t="n">
-        <v>2576</v>
+        <v>4557</v>
       </c>
       <c r="F3" t="n">
-        <v>4557</v>
+        <v>0.00938655783701059</v>
       </c>
       <c r="G3" t="n">
-        <v>0.00938655783701059</v>
+        <v>0.141842409558945</v>
       </c>
       <c r="H3" t="n">
-        <v>0.141842409558945</v>
+        <v>1.76902173913043</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="n">
-        <v>7</v>
+      <c r="B4" s="1" t="n">
+        <v>41091</v>
       </c>
       <c r="C4" t="n">
-        <v>2012</v>
+        <v>158714</v>
       </c>
       <c r="D4" t="n">
-        <v>158714</v>
+        <v>4884</v>
       </c>
       <c r="E4" t="n">
-        <v>4884</v>
+        <v>8700</v>
       </c>
       <c r="F4" t="n">
-        <v>8700</v>
+        <v>0.0307723326234611</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0307723326234611</v>
+        <v>0.26892792247123</v>
       </c>
       <c r="H4" t="n">
-        <v>0.26892792247123</v>
+        <v>1.78132678132678</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="n">
-        <v>8</v>
+      <c r="B5" s="1" t="n">
+        <v>41122</v>
       </c>
       <c r="C5" t="n">
-        <v>2012</v>
+        <v>391909</v>
       </c>
       <c r="D5" t="n">
-        <v>391909</v>
+        <v>12912</v>
       </c>
       <c r="E5" t="n">
-        <v>12912</v>
+        <v>23316</v>
       </c>
       <c r="F5" t="n">
-        <v>23316</v>
+        <v>0.0329464237871547</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0329464237871547</v>
+        <v>0.669744281342393</v>
       </c>
       <c r="H5" t="n">
-        <v>0.669744281342393</v>
+        <v>1.80576208178439</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="n">
-        <v>8</v>
+      <c r="B6" s="1" t="n">
+        <v>41122</v>
       </c>
       <c r="C6" t="n">
-        <v>2012</v>
+        <v>275554</v>
       </c>
       <c r="D6" t="n">
-        <v>275554</v>
+        <v>3165</v>
       </c>
       <c r="E6" t="n">
-        <v>3165</v>
+        <v>5572</v>
       </c>
       <c r="F6" t="n">
-        <v>5572</v>
+        <v>0.0114859519368255</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0114859519368255</v>
+        <v>0.1641682659889</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1641682659889</v>
+        <v>1.76050552922591</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="n">
-        <v>8</v>
+      <c r="B7" s="1" t="n">
+        <v>41122</v>
       </c>
       <c r="C7" t="n">
-        <v>2012</v>
+        <v>154851</v>
       </c>
       <c r="D7" t="n">
-        <v>154851</v>
+        <v>3202</v>
       </c>
       <c r="E7" t="n">
-        <v>3202</v>
+        <v>5760</v>
       </c>
       <c r="F7" t="n">
-        <v>5760</v>
+        <v>0.0206779420216854</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0206779420216854</v>
+        <v>0.166087452668707</v>
       </c>
       <c r="H7" t="n">
-        <v>0.166087452668707</v>
+        <v>1.79887570268582</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="n">
-        <v>9</v>
+      <c r="B8" s="1" t="n">
+        <v>41153</v>
       </c>
       <c r="C8" t="n">
-        <v>2012</v>
+        <v>272639</v>
       </c>
       <c r="D8" t="n">
-        <v>272639</v>
+        <v>8898</v>
       </c>
       <c r="E8" t="n">
-        <v>8898</v>
+        <v>16507</v>
       </c>
       <c r="F8" t="n">
-        <v>16507</v>
+        <v>0.0326365633676767</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0326365633676767</v>
+        <v>0.568271809937412</v>
       </c>
       <c r="H8" t="n">
-        <v>0.568271809937412</v>
+        <v>1.85513598561474</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="n">
-        <v>9</v>
+      <c r="B9" s="1" t="n">
+        <v>41153</v>
       </c>
       <c r="C9" t="n">
-        <v>2012</v>
+        <v>220687</v>
       </c>
       <c r="D9" t="n">
-        <v>220687</v>
+        <v>2381</v>
       </c>
       <c r="E9" t="n">
-        <v>2381</v>
+        <v>4050</v>
       </c>
       <c r="F9" t="n">
-        <v>4050</v>
+        <v>0.01078903605559</v>
       </c>
       <c r="G9" t="n">
-        <v>0.01078903605559</v>
+        <v>0.152062843275003</v>
       </c>
       <c r="H9" t="n">
-        <v>0.152062843275003</v>
+        <v>1.70096598068039</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="n">
-        <v>9</v>
+      <c r="B10" s="1" t="n">
+        <v>41153</v>
       </c>
       <c r="C10" t="n">
-        <v>2012</v>
+        <v>169190</v>
       </c>
       <c r="D10" t="n">
-        <v>169190</v>
+        <v>4379</v>
       </c>
       <c r="E10" t="n">
-        <v>4379</v>
+        <v>7869</v>
       </c>
       <c r="F10" t="n">
-        <v>7869</v>
+        <v>0.0258821443347716</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0258821443347716</v>
+        <v>0.279665346787585</v>
       </c>
       <c r="H10" t="n">
-        <v>0.279665346787585</v>
+        <v>1.79698561315369</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" t="n">
-        <v>10</v>
+      <c r="B11" s="1" t="n">
+        <v>41183</v>
       </c>
       <c r="C11" t="n">
-        <v>2012</v>
+        <v>302514</v>
       </c>
       <c r="D11" t="n">
-        <v>302514</v>
+        <v>9373</v>
       </c>
       <c r="E11" t="n">
-        <v>9373</v>
+        <v>17675</v>
       </c>
       <c r="F11" t="n">
-        <v>17675</v>
+        <v>0.0309836900110408</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0309836900110408</v>
+        <v>0.656602451838879</v>
       </c>
       <c r="H11" t="n">
-        <v>0.656602451838879</v>
+        <v>1.8857356235997</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B12" t="n">
-        <v>10</v>
+      <c r="B12" s="1" t="n">
+        <v>41183</v>
       </c>
       <c r="C12" t="n">
-        <v>2012</v>
+        <v>238845</v>
       </c>
       <c r="D12" t="n">
-        <v>238845</v>
+        <v>2418</v>
       </c>
       <c r="E12" t="n">
-        <v>2418</v>
+        <v>4446</v>
       </c>
       <c r="F12" t="n">
-        <v>4446</v>
+        <v>0.0101237204044464</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0101237204044464</v>
+        <v>0.16938704028021</v>
       </c>
       <c r="H12" t="n">
-        <v>0.16938704028021</v>
+        <v>1.83870967741935</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" t="n">
-        <v>10</v>
+      <c r="B13" s="1" t="n">
+        <v>41183</v>
       </c>
       <c r="C13" t="n">
-        <v>2012</v>
+        <v>107102</v>
       </c>
       <c r="D13" t="n">
-        <v>107102</v>
+        <v>2484</v>
       </c>
       <c r="E13" t="n">
-        <v>2484</v>
+        <v>4505</v>
       </c>
       <c r="F13" t="n">
-        <v>4505</v>
+        <v>0.02319284420459</v>
       </c>
       <c r="G13" t="n">
-        <v>0.02319284420459</v>
+        <v>0.174010507880911</v>
       </c>
       <c r="H13" t="n">
-        <v>0.174010507880911</v>
+        <v>1.81360708534622</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B14" t="n">
-        <v>11</v>
+      <c r="B14" s="1" t="n">
+        <v>41214</v>
       </c>
       <c r="C14" t="n">
-        <v>2012</v>
+        <v>320574</v>
       </c>
       <c r="D14" t="n">
-        <v>320574</v>
+        <v>10350</v>
       </c>
       <c r="E14" t="n">
-        <v>10350</v>
+        <v>18778</v>
       </c>
       <c r="F14" t="n">
-        <v>18778</v>
+        <v>0.0322858372793801</v>
       </c>
       <c r="G14" t="n">
-        <v>0.0322858372793801</v>
+        <v>0.666580794744638</v>
       </c>
       <c r="H14" t="n">
-        <v>0.666580794744638</v>
+        <v>1.81429951690821</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B15" t="n">
-        <v>11</v>
+      <c r="B15" s="1" t="n">
+        <v>41214</v>
       </c>
       <c r="C15" t="n">
-        <v>2012</v>
+        <v>178820</v>
       </c>
       <c r="D15" t="n">
-        <v>178820</v>
+        <v>1994</v>
       </c>
       <c r="E15" t="n">
-        <v>1994</v>
+        <v>3407</v>
       </c>
       <c r="F15" t="n">
-        <v>3407</v>
+        <v>0.0111508779778548</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0111508779778548</v>
+        <v>0.128421459393315</v>
       </c>
       <c r="H15" t="n">
-        <v>0.128421459393315</v>
+        <v>1.7086258776329</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
         <v>10</v>
       </c>
-      <c r="B16" t="n">
-        <v>11</v>
+      <c r="B16" s="1" t="n">
+        <v>41214</v>
       </c>
       <c r="C16" t="n">
-        <v>2012</v>
+        <v>138235</v>
       </c>
       <c r="D16" t="n">
-        <v>138235</v>
+        <v>3183</v>
       </c>
       <c r="E16" t="n">
-        <v>3183</v>
+        <v>5947</v>
       </c>
       <c r="F16" t="n">
-        <v>5947</v>
+        <v>0.0230260064383116</v>
       </c>
       <c r="G16" t="n">
-        <v>0.0230260064383116</v>
+        <v>0.204997745862047</v>
       </c>
       <c r="H16" t="n">
-        <v>0.204997745862047</v>
+        <v>1.86836317939051</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
         <v>8</v>
       </c>
-      <c r="B17" t="n">
-        <v>12</v>
+      <c r="B17" s="1" t="n">
+        <v>41244</v>
       </c>
       <c r="C17" t="n">
-        <v>2012</v>
+        <v>309540</v>
       </c>
       <c r="D17" t="n">
-        <v>309540</v>
+        <v>11613</v>
       </c>
       <c r="E17" t="n">
-        <v>11613</v>
+        <v>19947</v>
       </c>
       <c r="F17" t="n">
-        <v>19947</v>
+        <v>0.037516960651289</v>
       </c>
       <c r="G17" t="n">
-        <v>0.037516960651289</v>
+        <v>0.582718651211802</v>
       </c>
       <c r="H17" t="n">
-        <v>0.582718651211802</v>
+        <v>1.71764401963317</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="B18" t="n">
-        <v>12</v>
+      <c r="B18" s="1" t="n">
+        <v>41244</v>
       </c>
       <c r="C18" t="n">
-        <v>2012</v>
+        <v>234466</v>
       </c>
       <c r="D18" t="n">
-        <v>234466</v>
+        <v>3158</v>
       </c>
       <c r="E18" t="n">
-        <v>3158</v>
+        <v>5672</v>
       </c>
       <c r="F18" t="n">
-        <v>5672</v>
+        <v>0.0134689038069486</v>
       </c>
       <c r="G18" t="n">
-        <v>0.0134689038069486</v>
+        <v>0.158462542024186</v>
       </c>
       <c r="H18" t="n">
-        <v>0.158462542024186</v>
+        <v>1.79607346421786</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
         <v>10</v>
       </c>
-      <c r="B19" t="n">
-        <v>12</v>
+      <c r="B19" s="1" t="n">
+        <v>41244</v>
       </c>
       <c r="C19" t="n">
-        <v>2012</v>
+        <v>245433</v>
       </c>
       <c r="D19" t="n">
-        <v>245433</v>
+        <v>5158</v>
       </c>
       <c r="E19" t="n">
-        <v>5158</v>
+        <v>9133</v>
       </c>
       <c r="F19" t="n">
-        <v>9133</v>
+        <v>0.0210159188047247</v>
       </c>
       <c r="G19" t="n">
-        <v>0.0210159188047247</v>
+        <v>0.258818806764012</v>
       </c>
       <c r="H19" t="n">
-        <v>0.258818806764012</v>
+        <v>1.77064753780535</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
         <v>8</v>
       </c>
-      <c r="B20" t="n">
-        <v>1</v>
+      <c r="B20" s="1" t="n">
+        <v>41275</v>
       </c>
       <c r="C20" t="n">
-        <v>2013</v>
+        <v>393556</v>
       </c>
       <c r="D20" t="n">
-        <v>393556</v>
+        <v>13793</v>
       </c>
       <c r="E20" t="n">
-        <v>13793</v>
+        <v>25424</v>
       </c>
       <c r="F20" t="n">
-        <v>25424</v>
+        <v>0.0350471089247782</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0350471089247782</v>
+        <v>0.639749536178108</v>
       </c>
       <c r="H20" t="n">
-        <v>0.639749536178108</v>
+        <v>1.84325382440368</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
         <v>9</v>
       </c>
-      <c r="B21" t="n">
-        <v>1</v>
+      <c r="B21" s="1" t="n">
+        <v>41275</v>
       </c>
       <c r="C21" t="n">
-        <v>2013</v>
+        <v>341664</v>
       </c>
       <c r="D21" t="n">
-        <v>341664</v>
+        <v>4360</v>
       </c>
       <c r="E21" t="n">
-        <v>4360</v>
+        <v>7257</v>
       </c>
       <c r="F21" t="n">
-        <v>7257</v>
+        <v>0.0127610752083919</v>
       </c>
       <c r="G21" t="n">
-        <v>0.0127610752083919</v>
+        <v>0.202226345083488</v>
       </c>
       <c r="H21" t="n">
-        <v>0.202226345083488</v>
+        <v>1.6644495412844</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
         <v>10</v>
       </c>
-      <c r="B22" t="n">
-        <v>1</v>
+      <c r="B22" s="1" t="n">
+        <v>41275</v>
       </c>
       <c r="C22" t="n">
-        <v>2013</v>
+        <v>164601</v>
       </c>
       <c r="D22" t="n">
-        <v>164601</v>
+        <v>3407</v>
       </c>
       <c r="E22" t="n">
-        <v>3407</v>
+        <v>6165</v>
       </c>
       <c r="F22" t="n">
-        <v>6165</v>
+        <v>0.0206985376759558</v>
       </c>
       <c r="G22" t="n">
-        <v>0.0206985376759558</v>
+        <v>0.158024118738404</v>
       </c>
       <c r="H22" t="n">
-        <v>0.158024118738404</v>
+        <v>1.80950983269739</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
         <v>8</v>
       </c>
-      <c r="B23" t="n">
-        <v>2</v>
+      <c r="B23" s="1" t="n">
+        <v>41306</v>
       </c>
       <c r="C23" t="n">
-        <v>2013</v>
+        <v>247506</v>
       </c>
       <c r="D23" t="n">
-        <v>247506</v>
+        <v>9699</v>
       </c>
       <c r="E23" t="n">
-        <v>9699</v>
+        <v>18437</v>
       </c>
       <c r="F23" t="n">
-        <v>18437</v>
+        <v>0.039186928801726</v>
       </c>
       <c r="G23" t="n">
-        <v>0.039186928801726</v>
+        <v>0.684667513765354</v>
       </c>
       <c r="H23" t="n">
-        <v>0.684667513765354</v>
+        <v>1.90091762037323</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
         <v>9</v>
       </c>
-      <c r="B24" t="n">
-        <v>2</v>
+      <c r="B24" s="1" t="n">
+        <v>41306</v>
       </c>
       <c r="C24" t="n">
-        <v>2013</v>
+        <v>194983</v>
       </c>
       <c r="D24" t="n">
-        <v>194983</v>
+        <v>2071</v>
       </c>
       <c r="E24" t="n">
-        <v>2071</v>
+        <v>3915</v>
       </c>
       <c r="F24" t="n">
-        <v>3915</v>
+        <v>0.0106214387920998</v>
       </c>
       <c r="G24" t="n">
-        <v>0.0106214387920998</v>
+        <v>0.146195115064238</v>
       </c>
       <c r="H24" t="n">
-        <v>0.146195115064238</v>
+        <v>1.89039111540319</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
         <v>10</v>
       </c>
-      <c r="B25" t="n">
-        <v>2</v>
+      <c r="B25" s="1" t="n">
+        <v>41306</v>
       </c>
       <c r="C25" t="n">
-        <v>2013</v>
+        <v>107598</v>
       </c>
       <c r="D25" t="n">
-        <v>107598</v>
+        <v>2396</v>
       </c>
       <c r="E25" t="n">
-        <v>2396</v>
+        <v>4696</v>
       </c>
       <c r="F25" t="n">
-        <v>4696</v>
+        <v>0.0222680718972472</v>
       </c>
       <c r="G25" t="n">
-        <v>0.0222680718972472</v>
+        <v>0.169137371170408</v>
       </c>
       <c r="H25" t="n">
-        <v>0.169137371170408</v>
+        <v>1.95993322203673</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
         <v>8</v>
       </c>
-      <c r="B26" t="n">
-        <v>3</v>
+      <c r="B26" s="1" t="n">
+        <v>41334</v>
       </c>
       <c r="C26" t="n">
-        <v>2013</v>
+        <v>287633</v>
       </c>
       <c r="D26" t="n">
-        <v>287633</v>
+        <v>9679</v>
       </c>
       <c r="E26" t="n">
-        <v>9679</v>
+        <v>17362</v>
       </c>
       <c r="F26" t="n">
-        <v>17362</v>
+        <v>0.0336505199333873</v>
       </c>
       <c r="G26" t="n">
-        <v>0.0336505199333873</v>
+        <v>0.543641878229611</v>
       </c>
       <c r="H26" t="n">
-        <v>0.543641878229611</v>
+        <v>1.79378034920963</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
         <v>9</v>
       </c>
-      <c r="B27" t="n">
-        <v>3</v>
+      <c r="B27" s="1" t="n">
+        <v>41334</v>
       </c>
       <c r="C27" t="n">
-        <v>2013</v>
+        <v>304829</v>
       </c>
       <c r="D27" t="n">
-        <v>304829</v>
+        <v>3644</v>
       </c>
       <c r="E27" t="n">
-        <v>3644</v>
+        <v>6455</v>
       </c>
       <c r="F27" t="n">
-        <v>6455</v>
+        <v>0.0119542431986458</v>
       </c>
       <c r="G27" t="n">
-        <v>0.0119542431986458</v>
+        <v>0.204673107166929</v>
       </c>
       <c r="H27" t="n">
-        <v>0.204673107166929</v>
+        <v>1.77140504939627</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
         <v>10</v>
       </c>
-      <c r="B28" t="n">
-        <v>3</v>
+      <c r="B28" s="1" t="n">
+        <v>41334</v>
       </c>
       <c r="C28" t="n">
-        <v>2013</v>
+        <v>196145</v>
       </c>
       <c r="D28" t="n">
-        <v>196145</v>
+        <v>4481</v>
       </c>
       <c r="E28" t="n">
-        <v>4481</v>
+        <v>8265</v>
       </c>
       <c r="F28" t="n">
-        <v>8265</v>
+        <v>0.0228453440057101</v>
       </c>
       <c r="G28" t="n">
-        <v>0.0228453440057101</v>
+        <v>0.25168501460346</v>
       </c>
       <c r="H28" t="n">
-        <v>0.25168501460346</v>
+        <v>1.84445436286543</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
         <v>8</v>
       </c>
-      <c r="B29" t="n">
-        <v>4</v>
+      <c r="B29" s="1" t="n">
+        <v>41365</v>
       </c>
       <c r="C29" t="n">
-        <v>2013</v>
+        <v>567205</v>
       </c>
       <c r="D29" t="n">
-        <v>567205</v>
+        <v>18868</v>
       </c>
       <c r="E29" t="n">
-        <v>18868</v>
+        <v>34200</v>
       </c>
       <c r="F29" t="n">
-        <v>34200</v>
+        <v>0.0332648689627207</v>
       </c>
       <c r="G29" t="n">
-        <v>0.0332648689627207</v>
+        <v>0.621291448516579</v>
       </c>
       <c r="H29" t="n">
-        <v>0.621291448516579</v>
+        <v>1.812592749629</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
         <v>9</v>
       </c>
-      <c r="B30" t="n">
-        <v>4</v>
+      <c r="B30" s="1" t="n">
+        <v>41365</v>
       </c>
       <c r="C30" t="n">
-        <v>2013</v>
+        <v>429860</v>
       </c>
       <c r="D30" t="n">
-        <v>429860</v>
+        <v>4280</v>
       </c>
       <c r="E30" t="n">
-        <v>4280</v>
+        <v>7752</v>
       </c>
       <c r="F30" t="n">
-        <v>7752</v>
+        <v>0.0099567300981715</v>
       </c>
       <c r="G30" t="n">
-        <v>0.0099567300981715</v>
+        <v>0.140933188448747</v>
       </c>
       <c r="H30" t="n">
-        <v>0.140933188448747</v>
+        <v>1.81121495327103</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
         <v>10</v>
       </c>
-      <c r="B31" t="n">
-        <v>4</v>
+      <c r="B31" s="1" t="n">
+        <v>41365</v>
       </c>
       <c r="C31" t="n">
-        <v>2013</v>
+        <v>299231</v>
       </c>
       <c r="D31" t="n">
-        <v>299231</v>
+        <v>7221</v>
       </c>
       <c r="E31" t="n">
-        <v>7221</v>
+        <v>12994</v>
       </c>
       <c r="F31" t="n">
-        <v>12994</v>
+        <v>0.0241318579959964</v>
       </c>
       <c r="G31" t="n">
-        <v>0.0241318579959964</v>
+        <v>0.237775363034674</v>
       </c>
       <c r="H31" t="n">
-        <v>0.237775363034674</v>
+        <v>1.79947375709735</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
         <v>8</v>
       </c>
-      <c r="B32" t="n">
-        <v>5</v>
+      <c r="B32" s="1" t="n">
+        <v>41395</v>
       </c>
       <c r="C32" t="n">
-        <v>2013</v>
+        <v>526075</v>
       </c>
       <c r="D32" t="n">
-        <v>526075</v>
+        <v>18176</v>
       </c>
       <c r="E32" t="n">
-        <v>18176</v>
+        <v>33208</v>
       </c>
       <c r="F32" t="n">
-        <v>33208</v>
+        <v>0.0345502067195742</v>
       </c>
       <c r="G32" t="n">
-        <v>0.0345502067195742</v>
+        <v>0.640247983373842</v>
       </c>
       <c r="H32" t="n">
-        <v>0.640247983373842</v>
+        <v>1.82702464788732</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
         <v>9</v>
       </c>
-      <c r="B33" t="n">
-        <v>5</v>
+      <c r="B33" s="1" t="n">
+        <v>41395</v>
       </c>
       <c r="C33" t="n">
-        <v>2013</v>
+        <v>409789</v>
       </c>
       <c r="D33" t="n">
-        <v>409789</v>
+        <v>5413</v>
       </c>
       <c r="E33" t="n">
-        <v>5413</v>
+        <v>9790</v>
       </c>
       <c r="F33" t="n">
-        <v>9790</v>
+        <v>0.0132092369487712</v>
       </c>
       <c r="G33" t="n">
-        <v>0.0132092369487712</v>
+        <v>0.19067244355208</v>
       </c>
       <c r="H33" t="n">
-        <v>0.19067244355208</v>
+        <v>1.80860890448919</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
         <v>10</v>
       </c>
-      <c r="B34" t="n">
-        <v>5</v>
+      <c r="B34" s="1" t="n">
+        <v>41395</v>
       </c>
       <c r="C34" t="n">
-        <v>2013</v>
+        <v>228512</v>
       </c>
       <c r="D34" t="n">
-        <v>228512</v>
+        <v>4800</v>
       </c>
       <c r="E34" t="n">
-        <v>4800</v>
+        <v>8631</v>
       </c>
       <c r="F34" t="n">
-        <v>8631</v>
+        <v>0.0210054614199692</v>
       </c>
       <c r="G34" t="n">
-        <v>0.0210054614199692</v>
+        <v>0.169079573074078</v>
       </c>
       <c r="H34" t="n">
-        <v>0.169079573074078</v>
+        <v>1.798125</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
         <v>8</v>
       </c>
-      <c r="B35" t="n">
-        <v>6</v>
+      <c r="B35" s="1" t="n">
+        <v>41426</v>
       </c>
       <c r="C35" t="n">
-        <v>2013</v>
+        <v>554632</v>
       </c>
       <c r="D35" t="n">
-        <v>554632</v>
+        <v>19370</v>
       </c>
       <c r="E35" t="n">
-        <v>19370</v>
+        <v>35146</v>
       </c>
       <c r="F35" t="n">
-        <v>35146</v>
+        <v>0.0349240577536096</v>
       </c>
       <c r="G35" t="n">
-        <v>0.0349240577536096</v>
+        <v>0.560831547860328</v>
       </c>
       <c r="H35" t="n">
-        <v>0.560831547860328</v>
+        <v>1.8144553433144</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
         <v>9</v>
       </c>
-      <c r="B36" t="n">
-        <v>6</v>
+      <c r="B36" s="1" t="n">
+        <v>41426</v>
       </c>
       <c r="C36" t="n">
-        <v>2013</v>
+        <v>526473</v>
       </c>
       <c r="D36" t="n">
-        <v>526473</v>
+        <v>7412</v>
       </c>
       <c r="E36" t="n">
-        <v>7412</v>
+        <v>13017</v>
       </c>
       <c r="F36" t="n">
-        <v>13017</v>
+        <v>0.014078594723756</v>
       </c>
       <c r="G36" t="n">
-        <v>0.014078594723756</v>
+        <v>0.214604204065088</v>
       </c>
       <c r="H36" t="n">
-        <v>0.214604204065088</v>
+        <v>1.75620615218564</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
         <v>10</v>
       </c>
-      <c r="B37" t="n">
-        <v>6</v>
+      <c r="B37" s="1" t="n">
+        <v>41426</v>
       </c>
       <c r="C37" t="n">
-        <v>2013</v>
+        <v>307411</v>
       </c>
       <c r="D37" t="n">
-        <v>307411</v>
+        <v>7756</v>
       </c>
       <c r="E37" t="n">
-        <v>7756</v>
+        <v>13728</v>
       </c>
       <c r="F37" t="n">
-        <v>13728</v>
+        <v>0.0252300665883784</v>
       </c>
       <c r="G37" t="n">
-        <v>0.0252300665883784</v>
+        <v>0.224564248074585</v>
       </c>
       <c r="H37" t="n">
-        <v>0.224564248074585</v>
+        <v>1.76998452810727</v>
       </c>
     </row>
   </sheetData>
@@ -1406,66 +1405,66 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>19</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>21</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>23</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>24</v>
       </c>
-      <c r="S1" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>26</v>
+      <c r="A2" s="1" t="n">
+        <v>41395</v>
       </c>
       <c r="B2" t="n">
         <v>1164376</v>
@@ -1499,8 +1498,8 @@
       <c r="S2"/>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>27</v>
+      <c r="A3" s="1" t="n">
+        <v>41426</v>
       </c>
       <c r="B3" t="n">
         <v>1388516</v>

</xml_diff>